<commit_message>
add readme and clean data
</commit_message>
<xml_diff>
--- a/book.xlsx
+++ b/book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saifm\OneDrive\Desktop\Projects\pricetracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3D06FB-17B6-4C93-A0E8-073EE859E549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0576DD7-9326-41D0-9BBA-F9F3546169E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10580" windowWidth="19200" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="10810" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>ASIN</t>
-  </si>
-  <si>
-    <t>Bar Code</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Product Description</t>
   </si>
@@ -39,18 +33,6 @@
     <t xml:space="preserve"> Cost Price</t>
   </si>
   <si>
-    <t>Case Qty</t>
-  </si>
-  <si>
-    <t>B0B649DHQD</t>
-  </si>
-  <si>
-    <t>B0B647FY9L</t>
-  </si>
-  <si>
-    <t>B0B649HM4K</t>
-  </si>
-  <si>
     <t>Iphone 17 pro</t>
   </si>
   <si>
@@ -58,6 +40,12 @@
   </si>
   <si>
     <t>Google Pixel 9a</t>
+  </si>
+  <si>
+    <t>Apple Airpods Pro 3</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S25</t>
   </si>
 </sst>
 </file>
@@ -376,85 +364,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2">
+        <v>134000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B3">
+        <v>64000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>6287010580027</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>134000</v>
-      </c>
-      <c r="E2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B5" s="1">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
-        <v>6287010581017</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>64000</v>
-      </c>
-      <c r="E3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>6287010581055</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>43000</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
+      <c r="B6" s="1">
+        <v>75000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>